<commit_message>
Model console program initial structure
</commit_message>
<xml_diff>
--- a/ClotheModel/data.xlsx
+++ b/ClotheModel/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\DataSuite+\2017\LN\Logistic Regression\ClotheModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Personal\DiArE\2017\Noviembre\logistic_regression\ClotheModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Prenda</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Shaina</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1214582-54A3-4D41-8E3E-DB0ABFB9FCEF}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,8 +578,65 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>